<commit_message>
changed some project files
</commit_message>
<xml_diff>
--- a/Investigation/deeper_chatbot_experiments/Experiment_results.xlsx
+++ b/Investigation/deeper_chatbot_experiments/Experiment_results.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nathan\Documents\GitHub\Individual-Project\Investigation\deeper_chatbot_experiments\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE8654CC-5A60-475F-9D7F-3AE7AA11871A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,8 +24,46 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t>Bootbot</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Response time</t>
+  </si>
+  <si>
+    <t>Languages used</t>
+  </si>
+  <si>
+    <t>Extendibility</t>
+  </si>
+  <si>
+    <t>Range of platforms</t>
+  </si>
+  <si>
+    <t>Free</t>
+  </si>
+  <si>
+    <t>Bootbot scores /5</t>
+  </si>
+  <si>
+    <t>Javascript</t>
+  </si>
+  <si>
+    <t>Dialog flow</t>
+  </si>
+  <si>
+    <t>Pandora bot</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -330,13 +374,69 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "changed some project files"
This reverts commit 899f31950407b7fa18836df9115fedb5f87fa112.
</commit_message>
<xml_diff>
--- a/Investigation/deeper_chatbot_experiments/Experiment_results.xlsx
+++ b/Investigation/deeper_chatbot_experiments/Experiment_results.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nathan\Documents\GitHub\Individual-Project\Investigation\deeper_chatbot_experiments\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE8654CC-5A60-475F-9D7F-3AE7AA11871A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,46 +18,8 @@
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>Bootbot</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>Response time</t>
-  </si>
-  <si>
-    <t>Languages used</t>
-  </si>
-  <si>
-    <t>Extendibility</t>
-  </si>
-  <si>
-    <t>Range of platforms</t>
-  </si>
-  <si>
-    <t>Free</t>
-  </si>
-  <si>
-    <t>Bootbot scores /5</t>
-  </si>
-  <si>
-    <t>Javascript</t>
-  </si>
-  <si>
-    <t>Dialog flow</t>
-  </si>
-  <si>
-    <t>Pandora bot</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -374,69 +330,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:F6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>